<commit_message>
[update]: update protocol documentation and uplink tools.
</commit_message>
<xml_diff>
--- a/doc/BTBLE双模串口通信协议_V2.0.6.xlsx
+++ b/doc/BTBLE双模串口通信协议_V2.0.6.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20328" windowHeight="8820" firstSheet="2" activeTab="5"/>
+    <workbookView windowWidth="28128" windowHeight="12660" tabRatio="920" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="封面" sheetId="8" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="5">'CMD-BT'!$A$1:$K$196</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="8">'CMD-Call'!$A$1:$K$65</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">'CMD-LE'!$A$1:$K$165</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'CMD-System'!$A$1:$K$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'CMD-System'!$A$1:$K$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="13">'EVT-Audio'!$A$1:$K$45</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="11">'EVT-BT'!$A$1:$I$57</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="14">'EVT-Call'!$A$1:$K$61</definedName>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2621" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2630" uniqueCount="456">
   <si>
     <t>序号</t>
   </si>
@@ -1423,6 +1423,12 @@
   </si>
   <si>
     <t>按键模拟命令</t>
+  </si>
+  <si>
+    <t>Shell指令发送</t>
+  </si>
+  <si>
+    <t>DBG</t>
   </si>
 </sst>
 </file>
@@ -1435,7 +1441,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1486,21 +1492,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -1652,7 +1644,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1715,19 +1707,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1871,19 +1851,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2451,46 +2419,52 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="36" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="36" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2499,100 +2473,94 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2752,7 +2720,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2770,7 +2738,7 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2799,7 +2767,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2817,13 +2785,13 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5514,7 +5482,7 @@
   <sheetPr/>
   <dimension ref="A2:G199"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" topLeftCell="A172" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" topLeftCell="A181" workbookViewId="0">
       <selection activeCell="G138" sqref="G138"/>
     </sheetView>
   </sheetViews>
@@ -10858,10 +10826,10 @@
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:G27"/>
+  <dimension ref="B2:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -11174,8 +11142,67 @@
       <c r="F27" s="23"/>
       <c r="G27" s="24"/>
     </row>
+    <row r="28" ht="15.15"/>
+    <row r="29" ht="19.2" spans="2:7">
+      <c r="B29" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" ht="17.4" spans="2:7">
+      <c r="B30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" ht="17.4" spans="2:7">
+      <c r="B31" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="12"/>
+    </row>
+    <row r="32" ht="15.6" spans="2:7">
+      <c r="B32" s="13"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="17"/>
+    </row>
+    <row r="33" ht="16.35" spans="2:7">
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="24"/>
+    </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="22">
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="D6:G6"/>
@@ -11194,6 +11221,10 @@
     <mergeCell ref="D25:G25"/>
     <mergeCell ref="D26:G26"/>
     <mergeCell ref="D27:G27"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="D33:G33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -13809,10 +13840,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:G46"/>
+  <dimension ref="A2:G40"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -14326,24 +14357,6 @@
       <c r="E40" s="23"/>
       <c r="F40" s="23"/>
       <c r="G40" s="24"/>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="25"/>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="25"/>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="25"/>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="25"/>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="25"/>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="31">
@@ -14390,8 +14403,8 @@
   <sheetPr/>
   <dimension ref="A2:G195"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="J191" sqref="J191"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57:G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -17057,7 +17070,7 @@
   <sheetPr/>
   <dimension ref="A2:G160"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" topLeftCell="A133" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" topLeftCell="A85" workbookViewId="0">
       <selection activeCell="D92" sqref="D92:G92"/>
     </sheetView>
   </sheetViews>
@@ -19170,7 +19183,7 @@
   <sheetPr/>
   <dimension ref="A1:G164"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" topLeftCell="A7" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" topLeftCell="A134" workbookViewId="0">
       <selection activeCell="D36" sqref="D36:G36"/>
     </sheetView>
   </sheetViews>

</xml_diff>